<commit_message>
exchange of photos by h2 tags
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -89,6 +89,15 @@
   </si>
   <si>
     <t xml:space="preserve">(SEO ou accessiblité ?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">déplacer les scripts JS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cache pour les photos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API dépréciées</t>
   </si>
 </sst>
 </file>
@@ -301,10 +310,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.95"/>
@@ -385,6 +394,9 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="G3" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
@@ -516,6 +528,9 @@
       <c r="A14" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="B14" s="0" t="s">
+        <v>23</v>
+      </c>
       <c r="E14" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -525,6 +540,9 @@
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="B15" s="0" t="s">
+        <v>24</v>
+      </c>
       <c r="E15" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -533,6 +551,9 @@
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add keywords,description, title and robots
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -310,10 +310,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.95"/>
@@ -409,6 +409,9 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="G4" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
@@ -421,6 +424,9 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="G5" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
@@ -432,6 +438,9 @@
       <c r="E6" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add label to social
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -79,15 +79,21 @@
     <t xml:space="preserve">ajout google analytics</t>
   </si>
   <si>
+    <t xml:space="preserve">Accessibilité</t>
+  </si>
+  <si>
     <t xml:space="preserve">balise lang</t>
   </si>
   <si>
-    <t xml:space="preserve">sitecheckerpro</t>
+    <t xml:space="preserve">lighthouse</t>
   </si>
   <si>
     <t xml:space="preserve">keyword à 1px</t>
   </si>
   <si>
+    <t xml:space="preserve">black hat SEO</t>
+  </si>
+  <si>
     <t xml:space="preserve">(SEO ou accessiblité ?)</t>
   </si>
   <si>
@@ -98,6 +104,9 @@
   </si>
   <si>
     <t xml:space="preserve">API dépréciées</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label sur social</t>
   </si>
 </sst>
 </file>
@@ -310,7 +319,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -505,17 +514,17 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E12" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>9</v>
@@ -526,7 +535,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="E13" s="4" t="n">
         <f aca="false">FALSE()</f>
@@ -535,10 +547,10 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E14" s="4" t="n">
         <f aca="false">FALSE()</f>
@@ -547,10 +559,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E15" s="4" t="n">
         <f aca="false">FALSE()</f>
@@ -559,30 +571,39 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
change bootstrap & jquery but problem
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">tou les liens dans le footer</t>
   </si>
   <si>
-    <t xml:space="preserve">site non responsive, erreur js</t>
+    <t xml:space="preserve">pb Bootstrap Jquery</t>
   </si>
   <si>
     <t xml:space="preserve">sitemap,xml et robots,txt</t>
@@ -319,7 +319,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
return back with jquery bootstrap
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">pb Bootstrap Jquery</t>
   </si>
   <si>
-    <t xml:space="preserve">sitemap,xml et robots,txt</t>
+    <t xml:space="preserve">robots,txt</t>
   </si>
   <si>
     <t xml:space="preserve">meta canonical</t>
@@ -88,18 +88,9 @@
     <t xml:space="preserve">lighthouse</t>
   </si>
   <si>
-    <t xml:space="preserve">keyword à 1px</t>
-  </si>
-  <si>
-    <t xml:space="preserve">black hat SEO</t>
-  </si>
-  <si>
     <t xml:space="preserve">(SEO ou accessiblité ?)</t>
   </si>
   <si>
-    <t xml:space="preserve">déplacer les scripts JS</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cache pour les photos</t>
   </si>
   <si>
@@ -107,6 +98,12 @@
   </si>
   <si>
     <t xml:space="preserve">label sur social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minifier le css</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bug dans bloc.js</t>
   </si>
 </sst>
 </file>
@@ -316,19 +313,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.75390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="27" style="0" width="11.22"/>
@@ -490,6 +487,9 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="G9" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
@@ -535,12 +535,9 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="0" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="4" t="n">
@@ -550,65 +547,49 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="4" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="4" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1587,8 +1568,8 @@
     <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
change keywords and title
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -46,43 +46,64 @@
     <t xml:space="preserve">Balises sémantiques</t>
   </si>
   <si>
-    <t xml:space="preserve">il n’y a pas de balises sémantiques</t>
+    <t xml:space="preserve">Les balises sémantiques permettent une meilleur compréhension de la page par les robots de recherche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utiliser au maximum des balises sémantiques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.journalducm.com/web-semantique-seo/</t>
   </si>
   <si>
     <t xml:space="preserve">x</t>
   </si>
   <si>
-    <t xml:space="preserve">Images trop grandes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fichier images en bmp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">images a la place de h2 ou style</t>
+    <t xml:space="preserve">Taille et extension fichiers images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les fichiers sont trop lourds et les formats non optimisés pour le web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">préférer le format webp, redimensionner les images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">images a la place de h2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certaines images contiennent uniquement du texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remplacer ces images par du texte en dur dans le html</t>
   </si>
   <si>
     <t xml:space="preserve">meta keyword et description title</t>
   </si>
   <si>
-    <t xml:space="preserve">tou les liens dans le footer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pb Bootstrap Jquery</t>
+    <t xml:space="preserve">Les balises title et description sont vident et keywords ne correspond pas au site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tous les liens dans le footer</t>
   </si>
   <si>
     <t xml:space="preserve">robots,txt</t>
   </si>
   <si>
+    <t xml:space="preserve">Le fichier robots.txt ainsi que la balise meta robots est utilisé par les robots de recherches pour savoir quelle page indexer</t>
+  </si>
+  <si>
     <t xml:space="preserve">meta canonical</t>
   </si>
   <si>
-    <t xml:space="preserve">ajout google analytics</t>
-  </si>
-  <si>
     <t xml:space="preserve">Accessibilité</t>
   </si>
   <si>
-    <t xml:space="preserve">balise lang</t>
+    <t xml:space="preserve">balise lang non présente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette balise est utile pour les lecteurs d’écrans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajouter lang=’fr’ dans la balise html</t>
   </si>
   <si>
     <t xml:space="preserve">lighthouse</t>
@@ -100,10 +121,25 @@
     <t xml:space="preserve">label sur social</t>
   </si>
   <si>
+    <t xml:space="preserve">Les liens de réseaux sociaux n’ont pas de label, ce qui bloque le lecteur d’écran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajouter aria-label=’’ dans les balises liens</t>
+  </si>
+  <si>
     <t xml:space="preserve">minifier le css</t>
   </si>
   <si>
+    <t xml:space="preserve">Ces fichiers prennent de la place, les minifiers permet de gagner en rapidité</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bug dans bloc.js</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certains texte font 1px</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le fait d’avoir du texte de très petite taille ou de la meme couleur que le fond peu etre considéré comme du hack</t>
   </si>
 </sst>
 </file>
@@ -316,17 +352,17 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.75390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.79296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="100.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="54.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="63.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="27" style="0" width="11.22"/>
   </cols>
@@ -381,12 +417,18 @@
       <c r="C2" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
       <c r="E2" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
+      </c>
       <c r="G2" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -394,14 +436,20 @@
         <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="E3" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -409,14 +457,20 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="E4" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -424,14 +478,17 @@
         <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="E5" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -439,14 +496,11 @@
         <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E6" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -454,11 +508,17 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="E7" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -466,37 +526,43 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E8" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="E9" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="F9" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="G9" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E10" s="4" t="n">
         <f aca="false">FALSE()</f>
@@ -505,89 +571,65 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="4" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="4" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="4" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>9</v>
+        <v>38</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1565,9 +1607,9 @@
     <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
change page2 name, title page2
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -82,9 +82,6 @@
     <t xml:space="preserve">Les balises title et description sont vident et keywords ne correspond pas au site</t>
   </si>
   <si>
-    <t xml:space="preserve">tous les liens dans le footer</t>
-  </si>
-  <si>
     <t xml:space="preserve">robots,txt</t>
   </si>
   <si>
@@ -115,7 +112,10 @@
     <t xml:space="preserve">Cache pour les photos</t>
   </si>
   <si>
-    <t xml:space="preserve">API dépréciées</t>
+    <t xml:space="preserve">Vulnérabilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jquery 2,1,0 à jquery 3,5,1</t>
   </si>
   <si>
     <t xml:space="preserve">label sur social</t>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t xml:space="preserve">Le fait d’avoir du texte de très petite taille ou de la meme couleur que le fond peu etre considéré comme du hack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beaucoups de liens dans le footer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.rocktherankings.com/footer-links-seo/</t>
   </si>
 </sst>
 </file>
@@ -352,14 +358,14 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.79296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="100.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="100.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="54.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="63.85"/>
@@ -498,9 +504,15 @@
       <c r="B6" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="C6" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="E6" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -508,123 +520,116 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="0" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="E8" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="F8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E9" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="4" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1606,7 +1611,7 @@
     <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
link rel external and nofollow
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -145,7 +145,13 @@
     <t xml:space="preserve">Beaucoups de liens dans le footer</t>
   </si>
   <si>
+    <t xml:space="preserve">les liens des partenaires sont mis en external, les autres, en nofollow</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.rocktherankings.com/footer-links-seo/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chgt nom page2 en contact.html</t>
   </si>
 </sst>
 </file>
@@ -357,11 +363,11 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.8515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.95"/>
@@ -628,11 +634,18 @@
       <c r="B15" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="D15" s="0" t="s">
+        <v>41</v>
+      </c>
       <c r="F15" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>